<commit_message>
Reports on Ericsson KPIs, using different axis, title, and chartsheets.
</commit_message>
<xml_diff>
--- a/test input.xlsx
+++ b/test input.xlsx
@@ -8,6 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Metricas_Datos" sheetId="1" r:id="rId1"/>
+    <sheet name="Grafico1" sheetId="2" r:id="rId2"/>
+    <sheet name="Grafico2" sheetId="3" r:id="rId3"/>
+    <sheet name="Grafico3" sheetId="4" r:id="rId4"/>
+    <sheet name="Grafico4" sheetId="5" r:id="rId5"/>
+    <sheet name="Grafico5" sheetId="6" r:id="rId6"/>
+    <sheet name="Grafico6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -94,6 +100,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volumen de trafico de voz cursado &amp; Tasa de caidas de voz &amp; Tasa de fallos de accesibilidad de voz</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -103,11 +127,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Metricas_Datos'!$B$1</c:f>
+              <c:f>'Metricas_Datos'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cosa1</c:v>
+                  <c:v>cosa2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -143,27 +167,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Metricas_Datos'!$B$2:$B$8</c:f>
+              <c:f>'Metricas_Datos'!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -174,12 +198,9 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Metricas_Datos'!$C$1</c:f>
+              <c:f>'Metricas_Datos'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>cosa2</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -214,28 +235,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Metricas_Datos'!$C$2:$C$8</c:f>
+              <c:f>'Metricas_Datos'!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -245,12 +248,9 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Metricas_Datos'!$D$1</c:f>
+              <c:f>'Metricas_Datos'!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>cosa3</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -285,28 +285,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Metricas_Datos'!$D$2:$D$8</c:f>
+              <c:f>'Metricas_Datos'!$O$2:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -343,38 +325,1017 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volumen de trafico de datos &amp; Tasa de fallos de accesibilidad &amp; Tasa de caidas de datos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020003"/>
+        <c:axId val="50020004"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50020004"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020003"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="50020003"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="50020004"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tasa de Accesibilidad HSDPA &amp; Tasa Accesibilidad HSUPA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$M$2:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$K$2:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50030001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50030002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tasa de llamadas de voz originadas en 3G y que terminan en 2G</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50040001"/>
+        <c:axId val="50040002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50040001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50040002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50040002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50040001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volumen de SHO y Tasa de exito de SHO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$P$2:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$Q$2:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50050003"/>
+        <c:axId val="50050004"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50050001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50050002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50050004"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050003"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="50050003"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="50050004"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Volumen de IFHO y Tasa de Fallos de IFHO</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$R$2:$R$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metricas_Datos'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1-Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-Jan</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3-Jan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4-Jan</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5-Jan</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6-Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metricas_Datos'!$S$2:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50060003"/>
+        <c:axId val="50060004"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50060001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50060002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50060004"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060003"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="50060003"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="50060004"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -387,7 +1348,142 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308969" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -782,6 +1878,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>